<commit_message>
actualización gruplacs GI asociados al docotorado
</commit_message>
<xml_diff>
--- a/Gruoplac/Input/Base_Grupos.xlsx
+++ b/Gruoplac/Input/Base_Grupos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Networking\Documents\python\Pandas\Gruoplac\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655D2CF2-6FCC-4422-AC99-54470314BB45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196C51CC-A8DE-49BC-9546-AF5C9BF280CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1089,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>